<commit_message>
A B C D positions
</commit_message>
<xml_diff>
--- a/data/sheets/left_marker.xlsx
+++ b/data/sheets/left_marker.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -19,16 +20,94 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift/x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ey</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -44,6 +123,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,9 +178,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -165,7 +259,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -176,10 +270,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0471279470461363"/>
+          <c:x val="0.0471349120467071"/>
           <c:y val="0.0372151168381575"/>
-          <c:w val="0.860797778714332"/>
-          <c:h val="0.906048658524858"/>
+          <c:w val="0.860784659133805"/>
+          <c:h val="0.906000576978556"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -207,9 +301,4448 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="28800">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="28800">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="26"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="29"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="30"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="31"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="32"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="33"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="34"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="35"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="36"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="37"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="38"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="39"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="40"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="41"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="42"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="43"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="44"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="45"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="46"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="47"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="48"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="49"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="50"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="51"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="52"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="53"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="54"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="55"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="56"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="57"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="58"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="59"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="60"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="61"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="62"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="63"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="64"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="65"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="66"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="67"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="68"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="69"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="70"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="71"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="72"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="73"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="74"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="75"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="76"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="77"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="78"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="79"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="80"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="81"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="82"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="83"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="84"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="85"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="86"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="87"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="88"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="89"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="90"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="91"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="92"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="93"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="94"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="95"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="96"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="97"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="98"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="99"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="100"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="101"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="102"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="103"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="104"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="105"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="106"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="107"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="108"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="109"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="110"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="111"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="112"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="113"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="114"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="115"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="116"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="117"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="118"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="119"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="120"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="121"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="122"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="123"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="124"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="125"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="126"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="127"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="128"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="129"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="130"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="131"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="132"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="133"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="134"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="135"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="136"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="137"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="138"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="139"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="140"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="141"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="142"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="143"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="144"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="145"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="146"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="147"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="148"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="149"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="150"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="151"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="152"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="153"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="154"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="155"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="156"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="157"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="158"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="159"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="160"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="161"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="162"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="163"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="164"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="165"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="166"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="167"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="168"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="169"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="170"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="171"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="172"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="173"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="174"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="175"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="176"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="177"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="178"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="179"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="180"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="181"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="182"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="183"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="184"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="185"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="186"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="187"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="188"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="189"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="190"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="191"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="192"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="193"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="194"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="195"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="196"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="197"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="198"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="199"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="200"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="201"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="202"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="203"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="204"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="205"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="206"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="207"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="208"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="209"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="210"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="211"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="212"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="213"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="214"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="215"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="216"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="217"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="218"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="219"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="220"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="221"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="222"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="223"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="224"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="225"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="226"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="227"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="228"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="229"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="230"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="231"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="232"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="233"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="234"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="235"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="236"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="237"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="238"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="239"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="240"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="241"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="242"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="243"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="244"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="245"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="246"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="247"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="248"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="249"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="250"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="251"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="252"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="253"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="254"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="255"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="256"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="257"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="258"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="259"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="260"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="261"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="262"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="263"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="264"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="265"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="266"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="267"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="268"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="269"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="270"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="271"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="272"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="273"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="274"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="275"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="276"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="277"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="278"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="279"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="280"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="281"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="282"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="283"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="284"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="285"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="286"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="287"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="288"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="289"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="290"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="28800">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="291"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="292"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="293"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="294"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="295"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="296"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="297"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="298"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="299"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1"/>
+              </a:solidFill>
+              <a:ln w="28800">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="300"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="28800">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="301"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="302"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="303"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="304"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="305"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="306"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="307"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="308"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="309"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="310"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="311"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="312"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="313"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="314"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="315"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="316"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="317"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="318"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="319"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="320"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="321"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="322"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="323"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="324"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="325"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="326"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="327"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="328"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="329"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="330"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="331"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="332"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="333"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="334"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="335"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="336"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="337"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="338"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="339"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="340"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="341"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="342"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="343"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="344"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="345"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="346"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="347"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="348"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="349"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="350"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="351"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="352"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="353"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="354"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="355"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="356"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="357"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff950e"/>
+              </a:solidFill>
+              <a:ln w="6029941680">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="358"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c5000b">
+                  <a:alpha val="-25601112"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="4647817080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="359"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0084d1">
+                  <a:alpha val="-33901000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="12240360">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="360"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="361"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="362"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="363"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="364"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="365"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="366"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="314004"/>
+              </a:solidFill>
+              <a:ln w="1161954720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="367"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="aecf00"/>
+              </a:solidFill>
+              <a:ln w="4124252160">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="368"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4b1f6f">
+                  <a:alpha val="-628179704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="1772368920">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -218,6 +4751,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -226,6 +4760,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="290"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -234,6 +4769,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="299"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -242,12 +4778,14 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="300"/>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
             </c:dLbl>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1381,11 +5919,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="92666025"/>
-        <c:axId val="71838347"/>
+        <c:axId val="31919660"/>
+        <c:axId val="68864414"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92666025"/>
+        <c:axId val="31919660"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,14 +5958,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71838347"/>
+        <c:crossAx val="68864414"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71838347"/>
+        <c:axId val="68864414"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,7 +5980,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1471,7 +6009,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92666025"/>
+        <c:crossAx val="31919660"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1519,9 +6057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>743400</xdr:colOff>
+      <xdr:colOff>743040</xdr:colOff>
       <xdr:row>365</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1529,8 +6067,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="852480" y="51894000"/>
-        <a:ext cx="14521320" cy="7487280"/>
+        <a:off x="839880" y="51894000"/>
+        <a:ext cx="14304960" cy="7486920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1550,13 +6088,13 @@
   </sheetPr>
   <dimension ref="A1:A1500"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A320" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A320" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J369" activeCellId="0" sqref="J369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9069,4 +13607,241 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="6.93877551020408"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <f aca="false">B1/D1*A3/100</f>
+        <v>0.0366</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <f aca="false">ROUND(A4*B3/A3,1)</f>
+        <v>25.4</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="false">ROUND(B4*C3/B3,0)</f>
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="false">ROUND(C4*D3/C3,0)</f>
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">ROUND(D4*E3/D3,0)</f>
+        <v>47</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <f aca="false">ROUND(E4*F3/E3,0)</f>
+        <v>58</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <f aca="false">ROUND(F4*G3/F3,0)</f>
+        <v>63</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <f aca="false">ROUND(G4*H3/G3,0)</f>
+        <v>73</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <f aca="false">ROUND(H4*I3/H3,0)</f>
+        <v>78</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <f aca="false">ROUND(I4*J3/I3,0)</f>
+        <v>89</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <f aca="false">ROUND(J4*K3/J3,0)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="n">
+        <f aca="false">(B4+C4)/2</f>
+        <v>28.2</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="false">ROUND($F$1*B6,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">(D4+E4)/2</f>
+        <v>44.5</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">ROUND($F$1*D6,1)</f>
+        <v>1.6</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <f aca="false">(F4+G4)/2</f>
+        <v>60.5</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <f aca="false">ROUND($F$1*F6,1)</f>
+        <v>2.2</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <f aca="false">(H4+I4)/2</f>
+        <v>75.5</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <f aca="false">ROUND($F$1*H6,1)</f>
+        <v>2.8</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <f aca="false">(J4+K4)/2</f>
+        <v>91.5</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <f aca="false">ROUND($F$1*J6,1)</f>
+        <v>3.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>